<commit_message>
PS11 and Extra Credit
</commit_message>
<xml_diff>
--- a/FA2019/Gradesheet_Template.xlsx
+++ b/FA2019/Gradesheet_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Algorithms-CSCI-3104\FA2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1337036F-60EA-4810-B3BA-5B8705DC8B3D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB617B8F-703F-4182-9633-9C528E4CC2B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="9900" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="9900" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Homework" sheetId="6" r:id="rId1"/>
@@ -998,7 +998,7 @@
   <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1235,15 +1235,15 @@
         <v>9</v>
       </c>
       <c r="V4">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="X4">
         <f>SUM(B4:V4)</f>
-        <v>415.5</v>
+        <v>425.5</v>
       </c>
       <c r="Y4">
         <f>ROUND(X4/5.33,2)</f>
-        <v>77.95</v>
+        <v>79.83</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.35">
@@ -1308,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623DFFE4-181C-44F5-AA78-2FA59DC02884}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1365,15 +1365,17 @@
       <c r="F2">
         <v>89</v>
       </c>
-      <c r="G2">
-        <v>40.625</v>
-      </c>
       <c r="H2">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="J2">
         <f>ROUND(AVERAGE(C2:H2),2)</f>
-        <v>69.17</v>
+        <v>75.88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <v>40.625</v>
       </c>
     </row>
   </sheetData>
@@ -1385,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12B14349-324D-46DE-9104-92FEF3804702}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1426,11 +1428,11 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2">
         <f>Homework!Y4</f>
-        <v>77.95</v>
+        <v>79.83</v>
       </c>
       <c r="D2" s="2">
         <f>'Quiz Average'!J2</f>
-        <v>69.17</v>
+        <v>75.88</v>
       </c>
       <c r="E2" s="2">
         <v>70.75</v>
@@ -1439,12 +1441,12 @@
         <v>50.5</v>
       </c>
       <c r="G2" s="2">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2">
         <f>ROUND((D2*0.15+E2*0.25+C2*0.25+F2*0.25)/0.9,2)</f>
-        <v>66.86</v>
+        <v>68.5</v>
       </c>
       <c r="J2" s="2"/>
     </row>
@@ -1478,7 +1480,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2">
         <f>ROUND(C2*0.25+D2*0.15+E2*0.25+F2*0.25+G2*0.1, 2)</f>
-        <v>68.98</v>
+        <v>70.150000000000006</v>
       </c>
       <c r="J5" s="2"/>
     </row>

</xml_diff>